<commit_message>
Fix excel templates and use appendedPhrase instead of appendedNamePhrase
</commit_message>
<xml_diff>
--- a/templates/CoLDP flat.xlsx
+++ b/templates/CoLDP flat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/code/col/coldp/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFDA275-48B9-DA44-9799-82086E78F86A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB109390-4B49-7040-9469-7CE48E1E0F12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28960" windowHeight="16880" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4280" yWindow="2520" windowWidth="28960" windowHeight="16880" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="10" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
   <si>
     <t>taxonID</t>
   </si>
@@ -252,20 +252,20 @@
     <t>parentID</t>
   </si>
   <si>
-    <t>appendedNamePhrase</t>
-  </si>
-  <si>
     <t>scrutinizer</t>
   </si>
   <si>
     <t>scrutinizerDate</t>
+  </si>
+  <si>
+    <t>appendedPhrase</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -276,6 +276,11 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Helvetica"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -299,11 +304,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="L1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -985,8 +991,8 @@
       <c r="C1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
-        <v>72</v>
+      <c r="D1" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="E1" t="s">
         <v>38</v>
@@ -998,10 +1004,10 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" t="s">
         <v>73</v>
-      </c>
-      <c r="I1" t="s">
-        <v>74</v>
       </c>
       <c r="J1" t="s">
         <v>39</v>
@@ -1034,32 +1040,45 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="1025" width="11.5"/>
+    <col min="1" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="5" max="6" width="30.6640625" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="9" max="1028" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add taxon concept and species interaction relations
</commit_message>
<xml_diff>
--- a/templates/CoLDP flat.xlsx
+++ b/templates/CoLDP flat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/code/col/coldp/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB109390-4B49-7040-9469-7CE48E1E0F12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A992F901-A787-C54D-904A-C49BA628F81E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="2520" windowWidth="28960" windowHeight="16880" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1220" yWindow="460" windowWidth="28960" windowHeight="16880" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="10" r:id="rId1"/>
@@ -19,10 +19,11 @@
     <sheet name="TypeMaterial" sheetId="11" r:id="rId4"/>
     <sheet name="Taxon" sheetId="8" r:id="rId5"/>
     <sheet name="Synonym" sheetId="7" r:id="rId6"/>
-    <sheet name="Distribution" sheetId="2" r:id="rId7"/>
-    <sheet name="Media" sheetId="5" r:id="rId8"/>
-    <sheet name="VernacularName" sheetId="9" r:id="rId9"/>
-    <sheet name="Reference" sheetId="6" r:id="rId10"/>
+    <sheet name="TaxonRelation" sheetId="12" r:id="rId7"/>
+    <sheet name="Distribution" sheetId="2" r:id="rId8"/>
+    <sheet name="Media" sheetId="5" r:id="rId9"/>
+    <sheet name="VernacularName" sheetId="9" r:id="rId10"/>
+    <sheet name="Reference" sheetId="6" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="76">
   <si>
     <t>taxonID</t>
   </si>
@@ -259,6 +260,9 @@
   </si>
   <si>
     <t>appendedPhrase</t>
+  </si>
+  <si>
+    <t>relatedTaxonID</t>
   </si>
 </sst>
 </file>
@@ -729,6 +733,57 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="9" width="37" customWidth="1"/>
+    <col min="10" max="1025" width="11.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -1042,7 +1097,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -1093,6 +1148,44 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED3E88C-C718-344C-8ECD-1CFC7C1D5318}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="5" width="46.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -1133,7 +1226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
@@ -1184,55 +1277,4 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="9" width="37" customWidth="1"/>
-    <col min="10" max="1025" width="11.5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Use namePhrase instead of appendedPhrase
</commit_message>
<xml_diff>
--- a/templates/CoLDP flat.xlsx
+++ b/templates/CoLDP flat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/code/col/coldp/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A992F901-A787-C54D-904A-C49BA628F81E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB236EB-469B-7349-A5A1-B3269B43FB6B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="460" windowWidth="28960" windowHeight="16880" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1220" yWindow="460" windowWidth="28960" windowHeight="16880" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="10" r:id="rId1"/>
@@ -259,10 +259,10 @@
     <t>scrutinizerDate</t>
   </si>
   <si>
-    <t>appendedPhrase</t>
-  </si>
-  <si>
     <t>relatedTaxonID</t>
+  </si>
+  <si>
+    <t>namePhrase</t>
   </si>
 </sst>
 </file>
@@ -1026,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1047,7 +1047,7 @@
         <v>23</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
         <v>38</v>
@@ -1098,7 +1098,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1119,7 +1119,7 @@
         <v>23</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
         <v>38</v>
@@ -1151,7 +1151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED3E88C-C718-344C-8ECD-1CFC7C1D5318}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1163,7 +1163,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>25</v>

</xml_diff>